<commit_message>
Refactor: Ganti link excel
</commit_message>
<xml_diff>
--- a/Assets/UTS-5_Skor.xlsx
+++ b/Assets/UTS-5_Skor.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>Evan Nathanael Tanuri</t>
+  </si>
+  <si>
+    <t>1824067/52</t>
+  </si>
+  <si>
+    <t>Bryant Azraqi Mohammad</t>
   </si>
 </sst>
 </file>
@@ -1040,39 +1046,75 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="5" t="str">
+      <c r="A6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="5" t="str">
+        <v>5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="I6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="5" t="str">
+        <v>5</v>
+      </c>
+      <c r="M6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="P6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="Q6" s="5">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="5" t="str">
+        <v>5</v>
+      </c>
+      <c r="R6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="S6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="T6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="U6" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="V6" s="5">
         <f t="shared" si="4"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>

</xml_diff>